<commit_message>
perf: filtering, merging and featurization fucntions updated
</commit_message>
<xml_diff>
--- a/data/sort/custom-labels.xlsx
+++ b/data/sort/custom-labels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imac/Downloads/dev/oliynyk/CAF/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danila/Documents/GitHub/bobleesj/composition-analyzer-featurizer-app/data/sort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7270A5DB-B1FA-4645-9DF8-B10725AD2AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DFF8DB-41B3-3A44-BA9E-5C09A087727B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17320" yWindow="3860" windowWidth="19940" windowHeight="15980" activeTab="2" xr2:uid="{AFAA846F-C9BE-0C44-872E-0A64BC1D6AC0}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="18000" windowHeight="22500" activeTab="1" xr2:uid="{AFAA846F-C9BE-0C44-872E-0A64BC1D6AC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Binary" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="49">
   <si>
     <t>Fe</t>
   </si>
@@ -163,6 +163,27 @@
   </si>
   <si>
     <t>Element_D</t>
+  </si>
+  <si>
+    <t>Ba</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>Pr</t>
+  </si>
+  <si>
+    <t>Sr</t>
+  </si>
+  <si>
+    <t>Tl</t>
   </si>
 </sst>
 </file>
@@ -553,12 +574,12 @@
       <selection activeCell="B1" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="13.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
@@ -566,7 +587,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -582,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -590,7 +611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -598,7 +619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -606,7 +627,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -614,7 +635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -622,7 +643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -630,7 +651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -645,15 +666,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725E2BF0-9F7C-A046-A663-99B7642B11AE}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="A1:C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -665,130 +686,111 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
+      <c r="A3" t="s">
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
@@ -797,8 +799,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>28</v>
+      <c r="A14" t="s">
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -808,8 +810,8 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>29</v>
+      <c r="A15" t="s">
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -819,9 +821,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
@@ -830,9 +830,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
@@ -841,9 +839,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
@@ -852,9 +848,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
@@ -863,9 +857,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
@@ -878,13 +870,9 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -892,16 +880,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400FB916-E258-D54B-AF7A-95BC3B4EDC70}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
@@ -915,7 +903,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -929,7 +917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -943,7 +931,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -957,7 +945,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -971,7 +959,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -985,7 +973,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -999,7 +987,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1013,7 +1001,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1027,7 +1015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1038,7 +1026,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1049,7 +1037,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1057,7 +1045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1065,7 +1053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1073,7 +1061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
@@ -1081,7 +1069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1089,7 +1077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
@@ -1097,7 +1085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
@@ -1105,7 +1093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1113,7 +1101,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
@@ -1127,14 +1115,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="842fee2d-b2cc-439f-a35b-e2ba2c54f32c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d103ac1e-cf17-436c-9a57-322643758598">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1367,21 +1353,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="842fee2d-b2cc-439f-a35b-e2ba2c54f32c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d103ac1e-cf17-436c-9a57-322643758598">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9122F342-36C7-4695-B3C9-8773EFE605B9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F85B1AA1-687D-46E9-94CB-354533AF2EE4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="842fee2d-b2cc-439f-a35b-e2ba2c54f32c"/>
-    <ds:schemaRef ds:uri="d103ac1e-cf17-436c-9a57-322643758598"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1406,9 +1391,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F85B1AA1-687D-46E9-94CB-354533AF2EE4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9122F342-36C7-4695-B3C9-8773EFE605B9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="842fee2d-b2cc-439f-a35b-e2ba2c54f32c"/>
+    <ds:schemaRef ds:uri="d103ac1e-cf17-436c-9a57-322643758598"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>